<commit_message>
feat(docs): update documents to add SALARIO field
- Updated diccionario_datos.xlsx to include SALARIO (NUMERIC(10,2))
- Updated normalizacion_tablas.xlsx with changes for SALARIO
- Updated PDM-Zoologico.png to reflect new field
</commit_message>
<xml_diff>
--- a/docs/diccionario_datos.xlsx
+++ b/docs/diccionario_datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Documents\GitHub - Projects\Doc-UP-AlejandroJaimes\BDI-GB-ZOO\Diccionario de Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Documents\GitHub - Projects\Doc-UP-AlejandroJaimes\BDI-GB-ZOO\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B4B787-CA6E-4881-991F-4BA2004CCDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3EB8FC-4231-417F-9EAD-1422FC69D928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DICCIONARIO DE DATOS" sheetId="12" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="125">
   <si>
     <t>Campo</t>
   </si>
@@ -452,6 +452,15 @@
   </si>
   <si>
     <t>IDCuidador</t>
+  </si>
+  <si>
+    <t>Salario</t>
+  </si>
+  <si>
+    <t>NUMERIC</t>
+  </si>
+  <si>
+    <t>(10,2)</t>
   </si>
 </sst>
 </file>
@@ -647,7 +656,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -677,8 +686,20 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -689,18 +710,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1156,401 +1166,401 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="32.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24" t="s">
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:8" ht="201.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="22" t="str">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="17" t="str">
         <f>CONCATENATE(A16,"_LINK")</f>
         <v>ANIMALES_LINK</v>
       </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
     </row>
     <row r="17" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="22" t="str">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="17" t="str">
         <f t="shared" ref="F17:F26" si="0">CONCATENATE(A17,"_LINK")</f>
         <v>CUIDADOR_LINK</v>
       </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="22" t="str">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="17" t="str">
         <f t="shared" si="0"/>
         <v>ESPECIALIDAD_LINK</v>
       </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="22" t="str">
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="17" t="str">
         <f t="shared" si="0"/>
         <v>ESPECIE_LINK</v>
       </c>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="22" t="str">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="17" t="str">
         <f t="shared" si="0"/>
         <v>FAMILIA_LINK</v>
       </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="22" t="str">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="17" t="str">
         <f t="shared" si="0"/>
         <v>ESTADO_CONSERVACION_LINK</v>
       </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="1:8" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="22" t="str">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="17" t="str">
         <f t="shared" si="0"/>
         <v>HABITAT_LINK</v>
       </c>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="22" t="str">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="17" t="str">
         <f t="shared" si="0"/>
         <v>UBICACIÓN_LINK</v>
       </c>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="22" t="str">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="17" t="str">
         <f t="shared" si="0"/>
         <v>CLIMA_LINK</v>
       </c>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="22" t="str">
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="17" t="str">
         <f t="shared" si="0"/>
         <v>VISITANTES_LINK</v>
       </c>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
     </row>
     <row r="26" spans="1:8" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="22" t="str">
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="17" t="str">
         <f t="shared" si="0"/>
         <v>HABITAT_VISITANTES_LINK</v>
       </c>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
     </row>
     <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="23"/>
+      <c r="B28" s="19"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
@@ -1577,19 +1587,18 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
     <mergeCell ref="B13:H13"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A14:H14"/>
@@ -1604,18 +1613,19 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:H21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F16:H16" location="ANIMALES!A1" display="ANIMALES!A1" xr:uid="{41D3153E-B36E-45D2-8E1F-398D0A801C50}"/>
@@ -2040,10 +2050,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="222" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="222" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2124,19 +2134,36 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D6" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2228,7 +2255,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat(docs): update data dictionary and table normalization
Updated diccionario_datos.xlsx with the addition of "tipo visitantes" table and its associated relationships
Updated normalizacion_tablas.xlsx for revised table normalization structurfeat(docs): update data dictionary and table normalization

Updated diccionario_datos.xlsx with the addition of "tipo visitantes"
table and its associated relationships
Updated normalizacion_tablas.xlsx for revised table normalization
	structuree
</commit_message>
<xml_diff>
--- a/docs/diccionario_datos.xlsx
+++ b/docs/diccionario_datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Documents\GitHub - Projects\Doc-UP-AlejandroJaimes\BDI-GB-ZOO\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3EB8FC-4231-417F-9EAD-1422FC69D928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9250BF-D185-4D3B-B89D-F577A70BA89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DICCIONARIO DE DATOS" sheetId="12" r:id="rId1"/>
@@ -23,8 +23,9 @@
     <sheet name="HABITAT" sheetId="7" r:id="rId8"/>
     <sheet name="UBICACION" sheetId="8" r:id="rId9"/>
     <sheet name="CLIMA" sheetId="9" r:id="rId10"/>
-    <sheet name="VISITANTES" sheetId="10" r:id="rId11"/>
-    <sheet name="HABITAT_VISITANTES" sheetId="11" r:id="rId12"/>
+    <sheet name="TIPO_VISITANTES" sheetId="13" r:id="rId11"/>
+    <sheet name="VISITANTES" sheetId="10" r:id="rId12"/>
+    <sheet name="HABITAT_VISITANTES" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="139">
   <si>
     <t>Campo</t>
   </si>
@@ -461,6 +462,48 @@
   </si>
   <si>
     <t>(10,2)</t>
+  </si>
+  <si>
+    <t>CostoBase</t>
+  </si>
+  <si>
+    <t>Costo base de entrada para acceder a cada hábitat del zoológico, expresado en moneda local. Este valor representa el precio estándar antes de aplicar descuentos según el tipo de visitante</t>
+  </si>
+  <si>
+    <t>Identificador único del tipo de visitante.</t>
+  </si>
+  <si>
+    <t>Nombre descriptivo del tipo de visitante (e.g., Adulto, Menor de edad, Estudiante).</t>
+  </si>
+  <si>
+    <t>Porcentaje de descuento aplicable a este tipo de visitante. Representado como un valor entre 0 y 100.</t>
+  </si>
+  <si>
+    <t>Descuento</t>
+  </si>
+  <si>
+    <t>(5,2)</t>
+  </si>
+  <si>
+    <t>TIPO_VISITANTES</t>
+  </si>
+  <si>
+    <t>Almacena los distintos tipos de visitantes que acceden al zoológico, como Adulto, Menor de edad y Estudiante, junto con el porcentaje de descuento aplicable a cada tipo. Esta información permite calcular tarifas ajustadas según el tipo de visitante.</t>
+  </si>
+  <si>
+    <t>IDTipoVisitantes</t>
+  </si>
+  <si>
+    <t>Identificador del tipo de visitantes.</t>
+  </si>
+  <si>
+    <t>CostoFinal</t>
+  </si>
+  <si>
+    <t>NOT NULL (DEFAULT)</t>
+  </si>
+  <si>
+    <t>Costo final calculada del descuento por el tipo de visitante, calculado con la funcion calcular_descuento() que aplica la formula Costo Final=Costo Base×(1−Descuento/100)</t>
   </si>
 </sst>
 </file>
@@ -656,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -686,20 +729,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -710,7 +742,37 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1153,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{339450DB-CBA5-4825-8615-F0DCB265D8CD}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="116" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:H17"/>
+    <sheetView topLeftCell="A22" zoomScale="116" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,42 +1228,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="32.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1274,30 +1336,30 @@
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1342,32 +1404,32 @@
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21" t="s">
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:8" ht="201.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
@@ -1379,12 +1441,12 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="17" t="str">
+      <c r="F16" s="25" t="str">
         <f>CONCATENATE(A16,"_LINK")</f>
         <v>ANIMALES_LINK</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
     </row>
     <row r="17" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
@@ -1396,12 +1458,12 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="17" t="str">
-        <f t="shared" ref="F17:F26" si="0">CONCATENATE(A17,"_LINK")</f>
+      <c r="F17" s="25" t="str">
+        <f t="shared" ref="F17:F27" si="0">CONCATENATE(A17,"_LINK")</f>
         <v>CUIDADOR_LINK</v>
       </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -1413,12 +1475,12 @@
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="17" t="str">
+      <c r="F18" s="25" t="str">
         <f t="shared" si="0"/>
         <v>ESPECIALIDAD_LINK</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -1430,12 +1492,12 @@
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="17" t="str">
+      <c r="F19" s="25" t="str">
         <f t="shared" si="0"/>
         <v>ESPECIE_LINK</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
     </row>
     <row r="20" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
@@ -1447,12 +1509,12 @@
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="17" t="str">
+      <c r="F20" s="25" t="str">
         <f t="shared" si="0"/>
         <v>FAMILIA_LINK</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
@@ -1464,12 +1526,12 @@
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="17" t="str">
+      <c r="F21" s="25" t="str">
         <f t="shared" si="0"/>
         <v>ESTADO_CONSERVACION_LINK</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:8" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
@@ -1481,12 +1543,12 @@
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="17" t="str">
+      <c r="F22" s="25" t="str">
         <f t="shared" si="0"/>
         <v>HABITAT_LINK</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
     </row>
     <row r="23" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
@@ -1498,12 +1560,12 @@
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="17" t="str">
+      <c r="F23" s="25" t="str">
         <f t="shared" si="0"/>
         <v>UBICACIÓN_LINK</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
     </row>
     <row r="24" spans="1:8" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -1515,92 +1577,110 @@
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="17" t="str">
+      <c r="F24" s="25" t="str">
         <f t="shared" si="0"/>
         <v>CLIMA_LINK</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-    </row>
-    <row r="25" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+    </row>
+    <row r="25" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>VISITANTES_LINK</v>
-      </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-    </row>
-    <row r="26" spans="1:8" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="25" t="str">
+        <f t="shared" ref="F25" si="1">CONCATENATE(A25,"_LINK")</f>
+        <v>TIPO_VISITANTES_LINK</v>
+      </c>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="17" t="str">
+      <c r="F26" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>VISITANTES_LINK</v>
+      </c>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+    </row>
+    <row r="27" spans="1:8" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="25" t="str">
         <f t="shared" si="0"/>
         <v>HABITAT_VISITANTES_LINK</v>
       </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-    </row>
-    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A28" s="19" t="s">
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+    </row>
+    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="A29" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="19"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="B29" s="23"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
+  <mergeCells count="41">
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:H24"/>
     <mergeCell ref="B13:H13"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="F15:H15"/>
@@ -1614,18 +1694,19 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="F20:H20"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:H25"/>
     <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F16:H16" location="ANIMALES!A1" display="ANIMALES!A1" xr:uid="{41D3153E-B36E-45D2-8E1F-398D0A801C50}"/>
@@ -1637,8 +1718,9 @@
     <hyperlink ref="F22:H22" location="HABITAT!A1" display="HABITAT!A1" xr:uid="{EA91EF00-DA2F-4E00-A5D4-0C1085EBEEBD}"/>
     <hyperlink ref="F23:H23" location="UBICACION!A1" display="UBICACION!A1" xr:uid="{D55219A8-4FD7-4064-9327-347592192A6E}"/>
     <hyperlink ref="F24:H24" location="CLIMA!A1" display="CLIMA!A1" xr:uid="{F64C0BF4-3B73-43FB-9793-F7181E1241EE}"/>
-    <hyperlink ref="F25:H25" location="VISITANTES!A1" display="VISITANTES!A1" xr:uid="{6A052436-EAC5-44FE-9A66-0894D7AFE2D5}"/>
-    <hyperlink ref="F26:H26" location="HABITAT_VISITANTES!A1" display="HABITAT_VISITANTES!A1" xr:uid="{5D5A4D0B-FAC0-4239-9056-4A34635EA186}"/>
+    <hyperlink ref="F26:H26" location="VISITANTES!A1" display="VISITANTES!A1" xr:uid="{6A052436-EAC5-44FE-9A66-0894D7AFE2D5}"/>
+    <hyperlink ref="F27:H27" location="HABITAT_VISITANTES!A1" display="HABITAT_VISITANTES!A1" xr:uid="{5D5A4D0B-FAC0-4239-9056-4A34635EA186}"/>
+    <hyperlink ref="F25:H25" location="TIPO_VISITANTES!A1" display="TIPO_VISITANTES!A1" xr:uid="{C6CAA7F9-AD1A-4879-B9E9-5DCA400104BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1723,6 +1805,99 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E833B78-DC58-45CB-81FE-BE4A0FF3FA6D}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -1730,12 +1905,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
@@ -1776,7 +1951,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -1794,20 +1969,20 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="A4" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>50</v>
+      <c r="D4" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1815,15 +1990,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="127" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1897,6 +2072,40 @@
       </c>
       <c r="E4" s="9" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2052,7 +2261,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="222" workbookViewId="0">
+    <sheetView zoomScale="222" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2140,7 +2349,7 @@
       <c r="B5" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="17" t="s">
         <v>124</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -2571,19 +2780,19 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="162" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -2637,26 +2846,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>41</v>
+    <row r="4" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>8</v>
@@ -2668,6 +2877,23 @@
         <v>112</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>